<commit_message>
Add new Excel file for teams data from February 25-26, 2023
</commit_message>
<xml_diff>
--- a/data/1FEB_25_26/teams_25_26_1FEB.xlsx
+++ b/data/1FEB_25_26/teams_25_26_1FEB.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,11 +579,6 @@
           <t>PJ</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>JORNADA</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -597,94 +592,91 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7423580786026202</v>
+        <v>0.9512519662615976</v>
       </c>
       <c r="D2" t="n">
-        <v>1.033057851239669</v>
+        <v>0.9400072138474762</v>
       </c>
       <c r="E2" t="n">
-        <v>82.32445520581115</v>
+        <v>107.5526035313398</v>
       </c>
       <c r="F2" t="n">
-        <v>113.7512639029323</v>
+        <v>104.739862784433</v>
       </c>
       <c r="G2" t="n">
-        <v>-31.4268086971211</v>
+        <v>2.81274074690679</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2093023255813954</v>
+        <v>0.3081023331468066</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7419354838709677</v>
+        <v>0.7339337096595161</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4324324324324325</v>
+        <v>0.5249530579759746</v>
       </c>
       <c r="K2" t="n">
-        <v>200</v>
+        <v>2425</v>
       </c>
       <c r="L2" t="n">
-        <v>68</v>
+        <v>1010</v>
       </c>
       <c r="M2" t="n">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="N2" t="n">
-        <v>33</v>
+        <v>405</v>
       </c>
       <c r="O2" t="n">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="P2" t="n">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="Q2" t="n">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="R2" t="n">
-        <v>15</v>
+        <v>240</v>
       </c>
       <c r="S2" t="n">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="T2" t="n">
-        <v>23</v>
+        <v>294</v>
       </c>
       <c r="U2" t="n">
-        <v>18</v>
+        <v>195</v>
       </c>
       <c r="V2" t="n">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="W2" t="n">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="X2" t="n">
-        <v>25</v>
+        <v>244</v>
       </c>
       <c r="Y2" t="n">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="Z2" t="n">
-        <v>90</v>
+        <v>991</v>
       </c>
       <c r="AA2" t="n">
-        <v>91.59999999999999</v>
+        <v>1064.6</v>
       </c>
       <c r="AB2" t="n">
-        <v>82.59999999999999</v>
+        <v>938.6</v>
       </c>
       <c r="AC2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AMICS CASTELLÓ</t>
+          <t>CAJA RURAL CB ZAMORA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -693,94 +685,91 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.033057851239669</v>
+        <v>0.9675437305763718</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7423580786026202</v>
+        <v>0.9818680415844911</v>
       </c>
       <c r="E3" t="n">
-        <v>113.7512639029323</v>
+        <v>109.2441684077458</v>
       </c>
       <c r="F3" t="n">
-        <v>82.32445520581115</v>
+        <v>112.3086861517812</v>
       </c>
       <c r="G3" t="n">
-        <v>31.4268086971211</v>
+        <v>-3.064517744035398</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2580645161290323</v>
+        <v>0.3299206588430727</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.6783094234048547</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5675675675675675</v>
+        <v>0.5137710864657896</v>
       </c>
       <c r="K3" t="n">
-        <v>200</v>
+        <v>2622.766666666666</v>
       </c>
       <c r="L3" t="n">
-        <v>90</v>
+        <v>1127</v>
       </c>
       <c r="M3" t="n">
-        <v>24</v>
+        <v>282</v>
       </c>
       <c r="N3" t="n">
-        <v>39</v>
+        <v>558</v>
       </c>
       <c r="O3" t="n">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="P3" t="n">
-        <v>24</v>
+        <v>271</v>
       </c>
       <c r="Q3" t="n">
-        <v>15</v>
+        <v>236</v>
       </c>
       <c r="R3" t="n">
-        <v>23</v>
+        <v>322</v>
       </c>
       <c r="S3" t="n">
-        <v>8</v>
+        <v>136</v>
       </c>
       <c r="T3" t="n">
-        <v>34</v>
+        <v>312</v>
       </c>
       <c r="U3" t="n">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="V3" t="n">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="W3" t="n">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="X3" t="n">
-        <v>20</v>
+        <v>271</v>
       </c>
       <c r="Y3" t="n">
-        <v>25</v>
+        <v>295</v>
       </c>
       <c r="Z3" t="n">
-        <v>68</v>
+        <v>1151</v>
       </c>
       <c r="AA3" t="n">
-        <v>87.12</v>
+        <v>1166.68</v>
       </c>
       <c r="AB3" t="n">
-        <v>79.12</v>
+        <v>1030.68</v>
       </c>
       <c r="AC3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C.B. NATURAVIA MORÓN</t>
+          <t>CLUB OURENSE BALONCESTO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -789,94 +778,91 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.7621189405297352</v>
+        <v>0.9573571169651589</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9700392927308448</v>
+        <v>0.9534064698182326</v>
       </c>
       <c r="E4" t="n">
-        <v>89.65314520870078</v>
+        <v>113.1431250102263</v>
       </c>
       <c r="F4" t="n">
-        <v>113.7672811059908</v>
+        <v>108.0851073073915</v>
       </c>
       <c r="G4" t="n">
-        <v>-24.11413589729001</v>
+        <v>5.058017702834809</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2926829268292683</v>
+        <v>0.3997226683101379</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6734427124667767</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4459459459459459</v>
+        <v>0.5271279462376859</v>
       </c>
       <c r="K4" t="n">
-        <v>200</v>
+        <v>2200</v>
       </c>
       <c r="L4" t="n">
-        <v>61</v>
+        <v>920</v>
       </c>
       <c r="M4" t="n">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="N4" t="n">
-        <v>31</v>
+        <v>464</v>
       </c>
       <c r="O4" t="n">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="P4" t="n">
-        <v>30</v>
+        <v>248</v>
       </c>
       <c r="Q4" t="n">
-        <v>10</v>
+        <v>195</v>
       </c>
       <c r="R4" t="n">
-        <v>16</v>
+        <v>292</v>
       </c>
       <c r="S4" t="n">
-        <v>12</v>
+        <v>147</v>
       </c>
       <c r="T4" t="n">
-        <v>21</v>
+        <v>231</v>
       </c>
       <c r="U4" t="n">
+        <v>155</v>
+      </c>
+      <c r="V4" t="n">
+        <v>81</v>
+      </c>
+      <c r="W4" t="n">
+        <v>120</v>
+      </c>
+      <c r="X4" t="n">
+        <v>258</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>253</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>890</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>960.48</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>813.48</v>
+      </c>
+      <c r="AC4" t="n">
         <v>11</v>
-      </c>
-      <c r="V4" t="n">
-        <v>6</v>
-      </c>
-      <c r="W4" t="n">
-        <v>12</v>
-      </c>
-      <c r="X4" t="n">
-        <v>24</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>19</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>79</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>80.03999999999999</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>68.03999999999999</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAJA RURAL CB ZAMORA</t>
+          <t>FIBWI MALLORCA BASQUET PALMA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -885,94 +871,91 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8707723372034325</v>
+        <v>0.9398612686209228</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9069212410501194</v>
+        <v>0.9323048624933717</v>
       </c>
       <c r="E5" t="n">
-        <v>90.50367261280167</v>
+        <v>105.1046148735883</v>
       </c>
       <c r="F5" t="n">
-        <v>100.2638522427441</v>
+        <v>108.3485499653878</v>
       </c>
       <c r="G5" t="n">
-        <v>-9.7601796299424</v>
+        <v>-3.24393509179954</v>
       </c>
       <c r="H5" t="n">
-        <v>0.125</v>
+        <v>0.2942941014703973</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7647058823529411</v>
+        <v>0.5835330448156171</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5</v>
+        <v>0.4378127879834504</v>
       </c>
       <c r="K5" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L5" t="n">
-        <v>69</v>
+        <v>944</v>
       </c>
       <c r="M5" t="n">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="N5" t="n">
-        <v>35</v>
+        <v>422</v>
       </c>
       <c r="O5" t="n">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="P5" t="n">
-        <v>21</v>
+        <v>325</v>
       </c>
       <c r="Q5" t="n">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="R5" t="n">
-        <v>21</v>
+        <v>234</v>
       </c>
       <c r="S5" t="n">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="T5" t="n">
-        <v>26</v>
+        <v>209</v>
       </c>
       <c r="U5" t="n">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="V5" t="n">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="W5" t="n">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="X5" t="n">
-        <v>21</v>
+        <v>267</v>
       </c>
       <c r="Y5" t="n">
-        <v>23</v>
+        <v>245</v>
       </c>
       <c r="Z5" t="n">
-        <v>76</v>
+        <v>973</v>
       </c>
       <c r="AA5" t="n">
-        <v>79.24000000000001</v>
+        <v>1005.96</v>
       </c>
       <c r="AB5" t="n">
-        <v>76.24000000000001</v>
+        <v>898.96</v>
       </c>
       <c r="AC5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CLUB OURENSE BALONCESTO</t>
+          <t>FLEXICAR FUENLABRADA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -981,94 +964,91 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.088362068965517</v>
+        <v>0.9740704029015607</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8228133453561768</v>
+        <v>0.9862955721403316</v>
       </c>
       <c r="E6" t="n">
-        <v>133.245382585752</v>
+        <v>105.0514592687998</v>
       </c>
       <c r="F6" t="n">
-        <v>92.73373983739837</v>
+        <v>111.196304480828</v>
       </c>
       <c r="G6" t="n">
-        <v>40.51164274835362</v>
+        <v>-6.14484521202821</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5483870967741935</v>
+        <v>0.2022151330737098</v>
       </c>
       <c r="I6" t="n">
-        <v>0.75</v>
+        <v>0.7021911244793771</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6619718309859155</v>
+        <v>0.460900947380439</v>
       </c>
       <c r="K6" t="n">
-        <v>200</v>
+        <v>2200</v>
       </c>
       <c r="L6" t="n">
+        <v>884</v>
+      </c>
+      <c r="M6" t="n">
+        <v>208</v>
+      </c>
+      <c r="N6" t="n">
+        <v>384</v>
+      </c>
+      <c r="O6" t="n">
         <v>101</v>
       </c>
-      <c r="M6" t="n">
-        <v>28</v>
-      </c>
-      <c r="N6" t="n">
-        <v>50</v>
-      </c>
-      <c r="O6" t="n">
-        <v>9</v>
-      </c>
       <c r="P6" t="n">
-        <v>21</v>
+        <v>281</v>
       </c>
       <c r="Q6" t="n">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="R6" t="n">
-        <v>20</v>
+        <v>243</v>
       </c>
       <c r="S6" t="n">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="T6" t="n">
-        <v>30</v>
+        <v>249</v>
       </c>
       <c r="U6" t="n">
-        <v>16</v>
+        <v>180</v>
       </c>
       <c r="V6" t="n">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="W6" t="n">
-        <v>13</v>
+        <v>138</v>
       </c>
       <c r="X6" t="n">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="Y6" t="n">
-        <v>24</v>
+        <v>234</v>
       </c>
       <c r="Z6" t="n">
-        <v>73</v>
+        <v>952</v>
       </c>
       <c r="AA6" t="n">
-        <v>92.8</v>
+        <v>909.92</v>
       </c>
       <c r="AB6" t="n">
-        <v>75.8</v>
+        <v>843.92</v>
       </c>
       <c r="AC6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FLEXICAR FUENLABRADA</t>
+          <t>GRUPO ALEGA CANTABRIA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1077,94 +1057,91 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9700392927308448</v>
+        <v>0.9468769077138391</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7621189405297352</v>
+        <v>1.000842545791274</v>
       </c>
       <c r="E7" t="n">
-        <v>113.7672811059908</v>
+        <v>103.7187758344004</v>
       </c>
       <c r="F7" t="n">
-        <v>89.65314520870078</v>
+        <v>111.5832067140086</v>
       </c>
       <c r="G7" t="n">
-        <v>24.11413589729001</v>
+        <v>-7.864430879608207</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.2474592910009576</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7073170731707317</v>
+        <v>0.7243788572393841</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5540540540540541</v>
+        <v>0.4900989334046499</v>
       </c>
       <c r="K7" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L7" t="n">
-        <v>79</v>
+        <v>942</v>
       </c>
       <c r="M7" t="n">
-        <v>19</v>
+        <v>183</v>
       </c>
       <c r="N7" t="n">
-        <v>35</v>
+        <v>380</v>
       </c>
       <c r="O7" t="n">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="P7" t="n">
-        <v>24</v>
+        <v>323</v>
       </c>
       <c r="Q7" t="n">
-        <v>17</v>
+        <v>210</v>
       </c>
       <c r="R7" t="n">
-        <v>26</v>
+        <v>280</v>
       </c>
       <c r="S7" t="n">
+        <v>89</v>
+      </c>
+      <c r="T7" t="n">
+        <v>269</v>
+      </c>
+      <c r="U7" t="n">
+        <v>183</v>
+      </c>
+      <c r="V7" t="n">
+        <v>73</v>
+      </c>
+      <c r="W7" t="n">
+        <v>173</v>
+      </c>
+      <c r="X7" t="n">
+        <v>264</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>277</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1015</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>999.2</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>910.2</v>
+      </c>
+      <c r="AC7" t="n">
         <v>12</v>
-      </c>
-      <c r="T7" t="n">
-        <v>29</v>
-      </c>
-      <c r="U7" t="n">
-        <v>10</v>
-      </c>
-      <c r="V7" t="n">
-        <v>6</v>
-      </c>
-      <c r="W7" t="n">
-        <v>11</v>
-      </c>
-      <c r="X7" t="n">
-        <v>19</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>61</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>81.44</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>69.44</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GRUPO ALEGA CANTABRIA</t>
+          <t>GRUPO CAESA SEGUROS FC CARTAGENA CB</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1173,88 +1150,85 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8834388185654009</v>
+        <v>0.8370371045208113</v>
       </c>
       <c r="D8" t="n">
-        <v>1.147891083822744</v>
+        <v>0.9752759705370705</v>
       </c>
       <c r="E8" t="n">
-        <v>98.76179245283018</v>
+        <v>92.78846747946386</v>
       </c>
       <c r="F8" t="n">
-        <v>128.5116557083084</v>
+        <v>111.071334377164</v>
       </c>
       <c r="G8" t="n">
-        <v>-29.74986325547826</v>
+        <v>-18.28286689770015</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2758620689655172</v>
+        <v>0.2591198126800834</v>
       </c>
       <c r="I8" t="n">
-        <v>0.68</v>
+        <v>0.6892007480823271</v>
       </c>
       <c r="J8" t="n">
-        <v>0.462962962962963</v>
+        <v>0.478626712220329</v>
       </c>
       <c r="K8" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L8" t="n">
-        <v>67</v>
+        <v>845</v>
       </c>
       <c r="M8" t="n">
-        <v>18</v>
+        <v>213</v>
       </c>
       <c r="N8" t="n">
-        <v>36</v>
+        <v>421</v>
       </c>
       <c r="O8" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="P8" t="n">
-        <v>22</v>
+        <v>287</v>
       </c>
       <c r="Q8" t="n">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="R8" t="n">
-        <v>11</v>
+        <v>246</v>
       </c>
       <c r="S8" t="n">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="T8" t="n">
-        <v>17</v>
+        <v>279</v>
       </c>
       <c r="U8" t="n">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="V8" t="n">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="W8" t="n">
-        <v>13</v>
+        <v>193</v>
       </c>
       <c r="X8" t="n">
-        <v>21</v>
+        <v>288</v>
       </c>
       <c r="Y8" t="n">
-        <v>18</v>
+        <v>260</v>
       </c>
       <c r="Z8" t="n">
-        <v>86</v>
+        <v>1020</v>
       </c>
       <c r="AA8" t="n">
-        <v>75.84</v>
+        <v>1009.24</v>
       </c>
       <c r="AB8" t="n">
-        <v>67.84</v>
+        <v>910.24</v>
       </c>
       <c r="AC8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -1269,88 +1243,85 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.900805426027978</v>
+        <v>0.9514575645247937</v>
       </c>
       <c r="D9" t="n">
-        <v>1.009764758100311</v>
+        <v>1.016128889530707</v>
       </c>
       <c r="E9" t="n">
-        <v>100.7586533902323</v>
+        <v>109.539894324224</v>
       </c>
       <c r="F9" t="n">
-        <v>105.6665118439387</v>
+        <v>113.9913867847753</v>
       </c>
       <c r="G9" t="n">
-        <v>-4.907858453706339</v>
+        <v>-4.45149246055136</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2702702702702703</v>
+        <v>0.3626278251192095</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.6916783679123664</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5079365079365079</v>
+        <v>0.5174765361787116</v>
       </c>
       <c r="K9" t="n">
-        <v>200</v>
+        <v>2600</v>
       </c>
       <c r="L9" t="n">
-        <v>85</v>
+        <v>1107</v>
       </c>
       <c r="M9" t="n">
-        <v>23</v>
+        <v>253</v>
       </c>
       <c r="N9" t="n">
-        <v>39</v>
+        <v>480</v>
       </c>
       <c r="O9" t="n">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="P9" t="n">
-        <v>31</v>
+        <v>375</v>
       </c>
       <c r="Q9" t="n">
-        <v>12</v>
+        <v>214</v>
       </c>
       <c r="R9" t="n">
-        <v>19</v>
+        <v>287</v>
       </c>
       <c r="S9" t="n">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="T9" t="n">
-        <v>22</v>
+        <v>269</v>
       </c>
       <c r="U9" t="n">
-        <v>11</v>
+        <v>195</v>
       </c>
       <c r="V9" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="W9" t="n">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="X9" t="n">
-        <v>24</v>
+        <v>320</v>
       </c>
       <c r="Y9" t="n">
-        <v>21</v>
+        <v>286</v>
       </c>
       <c r="Z9" t="n">
-        <v>91</v>
+        <v>1157</v>
       </c>
       <c r="AA9" t="n">
-        <v>94.36</v>
+        <v>1163.28</v>
       </c>
       <c r="AB9" t="n">
-        <v>84.36</v>
+        <v>1010.28</v>
       </c>
       <c r="AC9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -1365,88 +1336,85 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9069212410501194</v>
+        <v>0.9742473931848826</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8707723372034325</v>
+        <v>0.9763965198759341</v>
       </c>
       <c r="E10" t="n">
-        <v>100.2638522427441</v>
+        <v>111.5880612488807</v>
       </c>
       <c r="F10" t="n">
-        <v>90.50367261280167</v>
+        <v>108.9074748544299</v>
       </c>
       <c r="G10" t="n">
-        <v>9.7601796299424</v>
+        <v>2.68058639445083</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2352941176470588</v>
+        <v>0.3340411731006543</v>
       </c>
       <c r="I10" t="n">
-        <v>0.875</v>
+        <v>0.7037098524732933</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5</v>
+        <v>0.5066736050766275</v>
       </c>
       <c r="K10" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L10" t="n">
-        <v>76</v>
+        <v>992</v>
       </c>
       <c r="M10" t="n">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="N10" t="n">
-        <v>29</v>
+        <v>397</v>
       </c>
       <c r="O10" t="n">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="P10" t="n">
-        <v>32</v>
+        <v>383</v>
       </c>
       <c r="Q10" t="n">
-        <v>15</v>
+        <v>188</v>
       </c>
       <c r="R10" t="n">
-        <v>20</v>
+        <v>247</v>
       </c>
       <c r="S10" t="n">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="T10" t="n">
-        <v>21</v>
+        <v>237</v>
       </c>
       <c r="U10" t="n">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="V10" t="n">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="W10" t="n">
-        <v>14</v>
+        <v>135</v>
       </c>
       <c r="X10" t="n">
-        <v>22</v>
+        <v>281</v>
       </c>
       <c r="Y10" t="n">
-        <v>20</v>
+        <v>252</v>
       </c>
       <c r="Z10" t="n">
-        <v>69</v>
+        <v>952</v>
       </c>
       <c r="AA10" t="n">
-        <v>83.8</v>
+        <v>1023.68</v>
       </c>
       <c r="AB10" t="n">
-        <v>75.8</v>
+        <v>889.6799999999999</v>
       </c>
       <c r="AC10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -1461,88 +1429,85 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7729468599033816</v>
+        <v>1.054891200941784</v>
       </c>
       <c r="D11" t="n">
-        <v>0.971261309207025</v>
+        <v>0.941463027939594</v>
       </c>
       <c r="E11" t="n">
-        <v>98.76543209876543</v>
+        <v>117.4644058050579</v>
       </c>
       <c r="F11" t="n">
-        <v>110.3385731559855</v>
+        <v>105.5403439880923</v>
       </c>
       <c r="G11" t="n">
-        <v>-11.57314105722007</v>
+        <v>11.92406181696556</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4390243902439024</v>
+        <v>0.2873231025268897</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.7195249475371793</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5428571428571428</v>
+        <v>0.5132407761328762</v>
       </c>
       <c r="K11" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L11" t="n">
-        <v>64</v>
+        <v>1057</v>
       </c>
       <c r="M11" t="n">
-        <v>17</v>
+        <v>232</v>
       </c>
       <c r="N11" t="n">
-        <v>44</v>
+        <v>442</v>
       </c>
       <c r="O11" t="n">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="P11" t="n">
-        <v>19</v>
+        <v>299</v>
       </c>
       <c r="Q11" t="n">
+        <v>236</v>
+      </c>
+      <c r="R11" t="n">
+        <v>284</v>
+      </c>
+      <c r="S11" t="n">
+        <v>103</v>
+      </c>
+      <c r="T11" t="n">
+        <v>280</v>
+      </c>
+      <c r="U11" t="n">
+        <v>210</v>
+      </c>
+      <c r="V11" t="n">
+        <v>80</v>
+      </c>
+      <c r="W11" t="n">
+        <v>136</v>
+      </c>
+      <c r="X11" t="n">
+        <v>261</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>249</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>949</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1001.96</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>898.96</v>
+      </c>
+      <c r="AC11" t="n">
         <v>12</v>
-      </c>
-      <c r="R11" t="n">
-        <v>20</v>
-      </c>
-      <c r="S11" t="n">
-        <v>18</v>
-      </c>
-      <c r="T11" t="n">
-        <v>20</v>
-      </c>
-      <c r="U11" t="n">
-        <v>15</v>
-      </c>
-      <c r="V11" t="n">
-        <v>6</v>
-      </c>
-      <c r="W11" t="n">
-        <v>11</v>
-      </c>
-      <c r="X11" t="n">
-        <v>18</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>23</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>73</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>82.8</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>64.8</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1557,94 +1522,91 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.747348119575699</v>
+        <v>0.9364464785328838</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9404005862237421</v>
+        <v>0.912738787130999</v>
       </c>
       <c r="E12" t="n">
-        <v>83.82909680908598</v>
+        <v>109.3600905991423</v>
       </c>
       <c r="F12" t="n">
-        <v>107.1229827490262</v>
+        <v>103.6488119754768</v>
       </c>
       <c r="G12" t="n">
-        <v>-23.29388593994018</v>
+        <v>5.711278623665486</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.3691903705356154</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.7012075707454528</v>
       </c>
       <c r="J12" t="n">
-        <v>0.4925373134328358</v>
+        <v>0.5331362049639178</v>
       </c>
       <c r="K12" t="n">
-        <v>200</v>
+        <v>2425</v>
       </c>
       <c r="L12" t="n">
-        <v>62</v>
+        <v>954</v>
       </c>
       <c r="M12" t="n">
-        <v>17</v>
+        <v>228</v>
       </c>
       <c r="N12" t="n">
-        <v>34</v>
+        <v>410</v>
       </c>
       <c r="O12" t="n">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="P12" t="n">
-        <v>28</v>
+        <v>361</v>
       </c>
       <c r="Q12" t="n">
-        <v>7</v>
+        <v>174</v>
       </c>
       <c r="R12" t="n">
-        <v>9</v>
+        <v>242</v>
       </c>
       <c r="S12" t="n">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="T12" t="n">
-        <v>24</v>
+        <v>281</v>
       </c>
       <c r="U12" t="n">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="V12" t="n">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="W12" t="n">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="X12" t="n">
-        <v>22</v>
+        <v>282</v>
       </c>
       <c r="Y12" t="n">
-        <v>17</v>
+        <v>244</v>
       </c>
       <c r="Z12" t="n">
-        <v>77</v>
+        <v>918</v>
       </c>
       <c r="AA12" t="n">
-        <v>82.96000000000001</v>
+        <v>1018.48</v>
       </c>
       <c r="AB12" t="n">
-        <v>73.96000000000001</v>
+        <v>872.48</v>
       </c>
       <c r="AC12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MONBUS OBRADOIRO</t>
+          <t>LEYMA CORUÑA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1653,94 +1615,91 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.8398247322297956</v>
+        <v>1.012409429236286</v>
       </c>
       <c r="D13" t="n">
-        <v>1.087533156498674</v>
+        <v>0.9032605386855272</v>
       </c>
       <c r="E13" t="n">
-        <v>96.964586846543</v>
+        <v>116.8171428770963</v>
       </c>
       <c r="F13" t="n">
-        <v>118.1556195965418</v>
+        <v>101.3998576680256</v>
       </c>
       <c r="G13" t="n">
-        <v>-21.19103274999878</v>
+        <v>15.41728520907067</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2972972972972973</v>
+        <v>0.3568934031211196</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.7339473181965137</v>
       </c>
       <c r="J13" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.5489441569094443</v>
       </c>
       <c r="K13" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L13" t="n">
-        <v>69</v>
+        <v>1096</v>
       </c>
       <c r="M13" t="n">
-        <v>17</v>
+        <v>257</v>
       </c>
       <c r="N13" t="n">
-        <v>40</v>
+        <v>472</v>
       </c>
       <c r="O13" t="n">
-        <v>8</v>
+        <v>119</v>
       </c>
       <c r="P13" t="n">
-        <v>25</v>
+        <v>352</v>
       </c>
       <c r="Q13" t="n">
-        <v>11</v>
+        <v>225</v>
       </c>
       <c r="R13" t="n">
-        <v>14</v>
+        <v>303</v>
       </c>
       <c r="S13" t="n">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="T13" t="n">
-        <v>23</v>
+        <v>305</v>
       </c>
       <c r="U13" t="n">
-        <v>16</v>
+        <v>206</v>
       </c>
       <c r="V13" t="n">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="W13" t="n">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="X13" t="n">
-        <v>18</v>
+        <v>267</v>
       </c>
       <c r="Y13" t="n">
-        <v>18</v>
+        <v>284</v>
       </c>
       <c r="Z13" t="n">
-        <v>82</v>
+        <v>924</v>
       </c>
       <c r="AA13" t="n">
-        <v>82.16</v>
+        <v>1084.32</v>
       </c>
       <c r="AB13" t="n">
-        <v>71.16</v>
+        <v>939.3199999999999</v>
       </c>
       <c r="AC13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MOVISTAR ESTUDIANTES</t>
+          <t>MELILLA CIUDAD DEL DEPORTE</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1749,94 +1708,91 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.087533156498674</v>
+        <v>0.8729988912785559</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8398247322297956</v>
+        <v>0.9760819931178699</v>
       </c>
       <c r="E14" t="n">
-        <v>118.1556195965418</v>
+        <v>97.76376405430427</v>
       </c>
       <c r="F14" t="n">
-        <v>96.964586846543</v>
+        <v>111.2044851953191</v>
       </c>
       <c r="G14" t="n">
-        <v>21.19103274999878</v>
+        <v>-13.44072114101482</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2068965517241379</v>
+        <v>0.2769717339322708</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7027027027027027</v>
+        <v>0.6938145450552399</v>
       </c>
       <c r="J14" t="n">
-        <v>0.4848484848484849</v>
+        <v>0.4895848616175565</v>
       </c>
       <c r="K14" t="n">
-        <v>200</v>
+        <v>2600</v>
       </c>
       <c r="L14" t="n">
-        <v>82</v>
+        <v>977</v>
       </c>
       <c r="M14" t="n">
-        <v>20</v>
+        <v>224</v>
       </c>
       <c r="N14" t="n">
-        <v>41</v>
+        <v>455</v>
       </c>
       <c r="O14" t="n">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="P14" t="n">
-        <v>22</v>
+        <v>338</v>
       </c>
       <c r="Q14" t="n">
-        <v>9</v>
+        <v>214</v>
       </c>
       <c r="R14" t="n">
-        <v>10</v>
+        <v>277</v>
       </c>
       <c r="S14" t="n">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="T14" t="n">
-        <v>26</v>
+        <v>318</v>
       </c>
       <c r="U14" t="n">
-        <v>17</v>
+        <v>195</v>
       </c>
       <c r="V14" t="n">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="W14" t="n">
-        <v>8</v>
+        <v>206</v>
       </c>
       <c r="X14" t="n">
-        <v>18</v>
+        <v>279</v>
       </c>
       <c r="Y14" t="n">
-        <v>18</v>
+        <v>280</v>
       </c>
       <c r="Z14" t="n">
-        <v>69</v>
+        <v>1123</v>
       </c>
       <c r="AA14" t="n">
-        <v>75.40000000000001</v>
+        <v>1120.88</v>
       </c>
       <c r="AB14" t="n">
-        <v>69.40000000000001</v>
+        <v>999.88</v>
       </c>
       <c r="AC14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ODILO FC CARTAGENA CB</t>
+          <t>MONBUS OBRADOIRO</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1845,94 +1801,91 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.8228133453561768</v>
+        <v>1.052819464442949</v>
       </c>
       <c r="D15" t="n">
-        <v>1.088362068965517</v>
+        <v>0.8830368757382004</v>
       </c>
       <c r="E15" t="n">
-        <v>92.73373983739837</v>
+        <v>117.7281925579684</v>
       </c>
       <c r="F15" t="n">
-        <v>133.245382585752</v>
+        <v>100.4779394014599</v>
       </c>
       <c r="G15" t="n">
-        <v>-40.51164274835362</v>
+        <v>17.25025315650852</v>
       </c>
       <c r="H15" t="n">
-        <v>0.25</v>
+        <v>0.2965957097272325</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.6747097196317394</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3380281690140845</v>
+        <v>0.4886998176960392</v>
       </c>
       <c r="K15" t="n">
-        <v>200</v>
+        <v>2425</v>
       </c>
       <c r="L15" t="n">
-        <v>73</v>
+        <v>1096</v>
       </c>
       <c r="M15" t="n">
-        <v>16</v>
+        <v>268</v>
       </c>
       <c r="N15" t="n">
-        <v>38</v>
+        <v>457</v>
       </c>
       <c r="O15" t="n">
-        <v>10</v>
+        <v>116</v>
       </c>
       <c r="P15" t="n">
-        <v>32</v>
+        <v>328</v>
       </c>
       <c r="Q15" t="n">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="R15" t="n">
-        <v>13</v>
+        <v>275</v>
       </c>
       <c r="S15" t="n">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="T15" t="n">
-        <v>14</v>
+        <v>260</v>
       </c>
       <c r="U15" t="n">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="V15" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="W15" t="n">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="X15" t="n">
-        <v>24</v>
+        <v>262</v>
       </c>
       <c r="Y15" t="n">
-        <v>17</v>
+        <v>271</v>
       </c>
       <c r="Z15" t="n">
-        <v>101</v>
+        <v>910</v>
       </c>
       <c r="AA15" t="n">
-        <v>88.72</v>
+        <v>1039</v>
       </c>
       <c r="AB15" t="n">
-        <v>78.72</v>
+        <v>930</v>
       </c>
       <c r="AC15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PALENCIA BALONCESTO</t>
+          <t>MOVISTAR ESTUDIANTES</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1941,94 +1894,91 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.009764758100311</v>
+        <v>1.012216685883531</v>
       </c>
       <c r="D16" t="n">
-        <v>0.900805426027978</v>
+        <v>0.9506764868181133</v>
       </c>
       <c r="E16" t="n">
-        <v>105.6665118439387</v>
+        <v>113.3089377132854</v>
       </c>
       <c r="F16" t="n">
-        <v>100.7586533902323</v>
+        <v>105.7696452003783</v>
       </c>
       <c r="G16" t="n">
-        <v>4.907858453706339</v>
+        <v>7.539292512907079</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1538461538461539</v>
+        <v>0.2939481215896992</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7297297297297297</v>
+        <v>0.7275296196622701</v>
       </c>
       <c r="J16" t="n">
-        <v>0.492063492063492</v>
+        <v>0.510732874392767</v>
       </c>
       <c r="K16" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L16" t="n">
-        <v>91</v>
+        <v>1041</v>
       </c>
       <c r="M16" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="N16" t="n">
-        <v>40</v>
+        <v>425</v>
       </c>
       <c r="O16" t="n">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="P16" t="n">
-        <v>24</v>
+        <v>340</v>
       </c>
       <c r="Q16" t="n">
-        <v>19</v>
+        <v>205</v>
       </c>
       <c r="R16" t="n">
-        <v>23</v>
+        <v>271</v>
       </c>
       <c r="S16" t="n">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="T16" t="n">
-        <v>27</v>
+        <v>280</v>
       </c>
       <c r="U16" t="n">
+        <v>181</v>
+      </c>
+      <c r="V16" t="n">
+        <v>84</v>
+      </c>
+      <c r="W16" t="n">
+        <v>142</v>
+      </c>
+      <c r="X16" t="n">
+        <v>267</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>278</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>960</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1026.24</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>917.24</v>
+      </c>
+      <c r="AC16" t="n">
         <v>12</v>
-      </c>
-      <c r="V16" t="n">
-        <v>10</v>
-      </c>
-      <c r="W16" t="n">
-        <v>16</v>
-      </c>
-      <c r="X16" t="n">
-        <v>21</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>85</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>90.12</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>86.12</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>REAL BETIS BALONCESTO</t>
+          <t>PALMER BASKET MALLORCA PALMA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2037,94 +1987,91 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9404005862237421</v>
+        <v>0.8133811627669387</v>
       </c>
       <c r="D17" t="n">
-        <v>0.747348119575699</v>
+        <v>0.9979501705229391</v>
       </c>
       <c r="E17" t="n">
-        <v>107.1229827490262</v>
+        <v>92.26037877167931</v>
       </c>
       <c r="F17" t="n">
-        <v>83.82909680908598</v>
+        <v>114.4298618096429</v>
       </c>
       <c r="G17" t="n">
-        <v>23.29388593994018</v>
+        <v>-22.16948303796356</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2941176470588235</v>
+        <v>0.2769931055394147</v>
       </c>
       <c r="I17" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.6352776093126483</v>
       </c>
       <c r="J17" t="n">
-        <v>0.5074626865671642</v>
+        <v>0.4386954986509536</v>
       </c>
       <c r="K17" t="n">
-        <v>200</v>
+        <v>2400</v>
       </c>
       <c r="L17" t="n">
-        <v>77</v>
+        <v>823</v>
       </c>
       <c r="M17" t="n">
+        <v>176</v>
+      </c>
+      <c r="N17" t="n">
+        <v>393</v>
+      </c>
+      <c r="O17" t="n">
+        <v>98</v>
+      </c>
+      <c r="P17" t="n">
+        <v>345</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>177</v>
+      </c>
+      <c r="R17" t="n">
+        <v>256</v>
+      </c>
+      <c r="S17" t="n">
+        <v>119</v>
+      </c>
+      <c r="T17" t="n">
+        <v>233</v>
+      </c>
+      <c r="U17" t="n">
+        <v>146</v>
+      </c>
+      <c r="V17" t="n">
+        <v>78</v>
+      </c>
+      <c r="W17" t="n">
+        <v>164</v>
+      </c>
+      <c r="X17" t="n">
+        <v>246</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>255</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>1053</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1014.64</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>895.64</v>
+      </c>
+      <c r="AC17" t="n">
         <v>12</v>
-      </c>
-      <c r="N17" t="n">
-        <v>34</v>
-      </c>
-      <c r="O17" t="n">
-        <v>10</v>
-      </c>
-      <c r="P17" t="n">
-        <v>28</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>23</v>
-      </c>
-      <c r="R17" t="n">
-        <v>27</v>
-      </c>
-      <c r="S17" t="n">
-        <v>10</v>
-      </c>
-      <c r="T17" t="n">
-        <v>24</v>
-      </c>
-      <c r="U17" t="n">
-        <v>11</v>
-      </c>
-      <c r="V17" t="n">
-        <v>11</v>
-      </c>
-      <c r="W17" t="n">
-        <v>8</v>
-      </c>
-      <c r="X17" t="n">
-        <v>17</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>22</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>62</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>81.88</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>71.88</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SILBÖ SAN PABLO BURGOS</t>
+          <t>SÚPER AGROPAL PALENCIA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2133,184 +2080,85 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.147891083822744</v>
+        <v>0.9579637140766728</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8834388185654009</v>
+        <v>0.8773321308156975</v>
       </c>
       <c r="E18" t="n">
-        <v>128.5116557083084</v>
+        <v>109.8786505247563</v>
       </c>
       <c r="F18" t="n">
-        <v>98.76179245283018</v>
+        <v>98.87132595144041</v>
       </c>
       <c r="G18" t="n">
-        <v>29.74986325547826</v>
+        <v>11.00732457331587</v>
       </c>
       <c r="H18" t="n">
-        <v>0.32</v>
+        <v>0.3229533556004144</v>
       </c>
       <c r="I18" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.7080125298888984</v>
       </c>
       <c r="J18" t="n">
-        <v>0.5370370370370371</v>
+        <v>0.5154989823007322</v>
       </c>
       <c r="K18" t="n">
-        <v>200</v>
+        <v>2600</v>
       </c>
       <c r="L18" t="n">
-        <v>86</v>
+        <v>1070</v>
       </c>
       <c r="M18" t="n">
-        <v>19</v>
+        <v>266</v>
       </c>
       <c r="N18" t="n">
-        <v>28</v>
+        <v>514</v>
       </c>
       <c r="O18" t="n">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="P18" t="n">
-        <v>27</v>
+        <v>366</v>
       </c>
       <c r="Q18" t="n">
-        <v>15</v>
+        <v>184</v>
       </c>
       <c r="R18" t="n">
-        <v>18</v>
+        <v>269</v>
       </c>
       <c r="S18" t="n">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="T18" t="n">
-        <v>21</v>
+        <v>291</v>
       </c>
       <c r="U18" t="n">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="V18" t="n">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="W18" t="n">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="X18" t="n">
-        <v>19</v>
+        <v>273</v>
       </c>
       <c r="Y18" t="n">
-        <v>21</v>
+        <v>265</v>
       </c>
       <c r="Z18" t="n">
-        <v>67</v>
+        <v>949</v>
       </c>
       <c r="AA18" t="n">
-        <v>74.92</v>
+        <v>1120.36</v>
       </c>
       <c r="AB18" t="n">
-        <v>66.92</v>
+        <v>972.36</v>
       </c>
       <c r="AC18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>UEMC REAL VALLADOLID BALONCESTO</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Liga Regular Único</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0.971261309207025</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.7729468599033816</v>
-      </c>
-      <c r="E19" t="n">
-        <v>110.3385731559855</v>
-      </c>
-      <c r="F19" t="n">
-        <v>98.76543209876543</v>
-      </c>
-      <c r="G19" t="n">
-        <v>11.57314105722007</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.3103448275862069</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.5609756097560976</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.4571428571428571</v>
-      </c>
-      <c r="K19" t="n">
-        <v>200</v>
-      </c>
-      <c r="L19" t="n">
-        <v>73</v>
-      </c>
-      <c r="M19" t="n">
         <v>13</v>
-      </c>
-      <c r="N19" t="n">
-        <v>23</v>
-      </c>
-      <c r="O19" t="n">
-        <v>12</v>
-      </c>
-      <c r="P19" t="n">
-        <v>34</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>11</v>
-      </c>
-      <c r="R19" t="n">
-        <v>14</v>
-      </c>
-      <c r="S19" t="n">
-        <v>9</v>
-      </c>
-      <c r="T19" t="n">
-        <v>23</v>
-      </c>
-      <c r="U19" t="n">
-        <v>18</v>
-      </c>
-      <c r="V19" t="n">
-        <v>8</v>
-      </c>
-      <c r="W19" t="n">
-        <v>12</v>
-      </c>
-      <c r="X19" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>18</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>64</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>75.16</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>66.16</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>